<commit_message>
Adding some withOUT replacement results. Experiments agree with before and look like a mix between logn and n. Need to rerun all experiments from scratch
</commit_message>
<xml_diff>
--- a/round_counts_old.xlsx
+++ b/round_counts_old.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/motiwari/Desktop/RandomForest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6110DE46-A70E-4A4D-900B-53CA4F738AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729724B5-52E6-9747-9795-E9E0FA6BF1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{B6551A33-E19F-6B46-8D1B-EB46F1BF4925}"/>
+    <workbookView xWindow="-15360" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{B6551A33-E19F-6B46-8D1B-EB46F1BF4925}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FC6165-C156-AC4B-8123-9772CFCE4A2A}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,11 +509,11 @@
         <v>58</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L17" si="0">AVERAGE(B3:K3)</f>
+        <f t="shared" ref="L3:L16" si="0">AVERAGE(B3:K3)</f>
         <v>80.7</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M17" si="1">STDEV(B3:K3)</f>
+        <f t="shared" ref="M3:M16" si="1">STDEV(B3:K3)</f>
         <v>15.832807008795932</v>
       </c>
     </row>
@@ -596,7 +596,7 @@
       <c r="K5">
         <v>106</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
         <f t="shared" si="0"/>
         <v>146.69999999999999</v>
       </c>
@@ -772,7 +772,7 @@
       <c r="K9">
         <v>139</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1">
         <f t="shared" si="0"/>
         <v>229.9</v>
       </c>
@@ -1133,6 +1133,102 @@
         <v>797.04428986098378</v>
       </c>
     </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>250000</v>
+      </c>
+      <c r="L20">
+        <v>819.2</v>
+      </c>
+      <c r="M20">
+        <v>862.37800000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>400000</v>
+      </c>
+      <c r="L21">
+        <v>1483.9</v>
+      </c>
+      <c r="M21">
+        <v>1612.96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>450000</v>
+      </c>
+      <c r="L22">
+        <v>1522.5</v>
+      </c>
+      <c r="M22">
+        <v>1447.1379999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>500000</v>
+      </c>
+      <c r="L23">
+        <v>1016.4</v>
+      </c>
+      <c r="M23">
+        <v>1238.55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>550000</v>
+      </c>
+      <c r="L24">
+        <v>964.3</v>
+      </c>
+      <c r="M24">
+        <v>1339.26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>600000</v>
+      </c>
+      <c r="L25">
+        <v>1363.6</v>
+      </c>
+      <c r="M25">
+        <v>1797.63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>700000</v>
+      </c>
+      <c r="L26">
+        <v>2968.3</v>
+      </c>
+      <c r="M26">
+        <v>2273.31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>800000</v>
+      </c>
+      <c r="L27">
+        <v>1910.7</v>
+      </c>
+      <c r="M27">
+        <v>1618.98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <v>2261.5</v>
+      </c>
+      <c r="M28">
+        <v>3352.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>